<commit_message>
webAPI: predict_more_row new endpoint
</commit_message>
<xml_diff>
--- a/DB séma train_excel.xlsx
+++ b/DB séma train_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\source\strabag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\strabag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1891F09-29BE-4E1A-86E2-16273ACECC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D4F208-8B01-42E5-BEC0-0907E7C83B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0692BD6E-48F9-45FE-A29D-EBA3E21B7AD2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>DB séma train_excel</t>
   </si>
@@ -174,9 +174,6 @@
     <t>magyarázat: ebben a táblában tároljuk a header szövegeket, azaz oszlop azonosítókat</t>
   </si>
   <si>
-    <t>users</t>
-  </si>
-  <si>
     <t>target</t>
   </si>
   <si>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t>headers</t>
+  </si>
+  <si>
+    <t>header_row</t>
+  </si>
+  <si>
+    <t>architects</t>
   </si>
 </sst>
 </file>
@@ -914,7 +917,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +931,9 @@
     <col min="9" max="9" width="21.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="12.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
@@ -955,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>45</v>
@@ -993,16 +998,19 @@
         <v>37</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S6" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1040,7 +1048,10 @@
       <c r="P7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1063,7 +1074,8 @@
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
-      <c r="Q8" s="7"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
@@ -1078,7 +1090,8 @@
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
-      <c r="Q9" s="7"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
@@ -1093,7 +1106,8 @@
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
-      <c r="Q10" s="7"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
@@ -1108,7 +1122,8 @@
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
       <c r="P11" s="22"/>
-      <c r="Q11" s="7"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
@@ -1123,7 +1138,8 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="10"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="10"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L13" s="1" t="s">
@@ -1135,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new DB DB séma Merkbau
</commit_message>
<xml_diff>
--- a/DB séma train_excel.xlsx
+++ b/DB séma train_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\strabag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1CE689-A34A-4C37-AEF2-8342E60CCF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8271DB74-16DC-4976-A6CE-D8DF2F096FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0692BD6E-48F9-45FE-A29D-EBA3E21B7AD2}"/>
+    <workbookView xWindow="9510" yWindow="615" windowWidth="14715" windowHeight="14985" xr2:uid="{0692BD6E-48F9-45FE-A29D-EBA3E21B7AD2}"/>
   </bookViews>
   <sheets>
     <sheet name="PostgreSQL" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="159">
   <si>
     <t>DB séma train_excel</t>
   </si>
@@ -215,9 +215,6 @@
     <t>hány db lett már bekategorizálva</t>
   </si>
   <si>
-    <t>JSON</t>
-  </si>
-  <si>
     <t>{"row_id":0, "main_cat_id": 1, "sub_cat_id": 2}</t>
   </si>
   <si>
@@ -507,6 +504,15 @@
   </si>
   <si>
     <t xml:space="preserve">SumText </t>
+  </si>
+  <si>
+    <t>FirstRowNumber</t>
+  </si>
+  <si>
+    <t>milyen sorszámmal kezdődik az első sor ID-je</t>
+  </si>
+  <si>
+    <t>TEXT</t>
   </si>
 </sst>
 </file>
@@ -740,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -810,11 +816,10 @@
     <xf numFmtId="49" fontId="1" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1348,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2964B59E-6EC2-4CDD-BD01-A4EE83B4F2B7}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="U34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA42" sqref="AA42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,15 +1404,15 @@
     <row r="3" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>28</v>
@@ -1417,19 +1422,19 @@
     </row>
     <row r="5" spans="1:23" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:23" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1437,34 +1442,34 @@
         <v>49</v>
       </c>
       <c r="H6" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="L6" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="L6" s="41" t="s">
+      <c r="M6" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="N6" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="O6" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="P6" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="P6" s="24" t="s">
-        <v>139</v>
-      </c>
       <c r="T6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1483,7 +1488,7 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N7" s="18" t="s">
         <v>12</v>
@@ -1493,12 +1498,12 @@
       </c>
       <c r="P7" s="5"/>
       <c r="T7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>11</v>
@@ -1512,7 +1517,7 @@
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N8" s="21"/>
       <c r="O8" s="18"/>
@@ -1520,7 +1525,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" s="36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="10"/>
@@ -1554,7 +1559,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="10"/>
@@ -1568,7 +1573,7 @@
     </row>
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="11"/>
@@ -1586,12 +1591,12 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1602,31 +1607,31 @@
         <v>30</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I17" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K17" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L17" s="41" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="M17" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -1637,14 +1642,14 @@
         <v>3</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="53" t="s">
-        <v>100</v>
+        <v>92</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>99</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>12</v>
@@ -1667,7 +1672,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="29"/>
       <c r="E19" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="46"/>
@@ -1829,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E30" s="18"/>
       <c r="F30" s="5"/>
@@ -1838,7 +1843,7 @@
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
       <c r="M30" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N30" s="18"/>
       <c r="O30" s="5"/>
@@ -1930,110 +1935,110 @@
       <c r="G38" s="18"/>
       <c r="H38" s="21"/>
       <c r="J38" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="2:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="K39" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="L39" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="M39" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="J39" s="49" t="s">
+      <c r="N39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="K39" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="L39" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="M39" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="N39" s="3" t="s">
+      <c r="O39" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="O39" s="3" t="s">
+      <c r="P39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="P39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Q39" s="3" t="s">
+      <c r="R39" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="T39" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="R39" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="S39" s="3" t="s">
+      <c r="U39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="V39" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="T39" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="U39" s="3" t="s">
+      <c r="W39" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="X39" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z39" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA39" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="V39" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="W39" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="X39" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y39" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z39" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA39" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="40" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" s="41" t="s">
+      <c r="G40" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="41" t="s">
+      <c r="H40" s="43" t="s">
         <v>108</v>
-      </c>
-      <c r="H40" s="43" t="s">
-        <v>109</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L40" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M40" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="N40" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="N40" s="18" t="s">
-        <v>64</v>
       </c>
       <c r="O40" s="18"/>
       <c r="P40" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q40" s="18"/>
       <c r="R40" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S40" s="18"/>
       <c r="T40" s="18"/>
@@ -2046,16 +2051,16 @@
       <c r="Y40" s="18"/>
       <c r="Z40" s="18"/>
       <c r="AA40" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B41" s="16"/>
       <c r="C41" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
@@ -2065,11 +2070,11 @@
       <c r="K41" s="27"/>
       <c r="L41" s="27"/>
       <c r="M41" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N41" s="18"/>
       <c r="O41" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P41" s="18"/>
       <c r="Q41" s="18"/>
@@ -2083,7 +2088,7 @@
       <c r="Y41" s="18"/>
       <c r="Z41" s="18"/>
       <c r="AA41" s="5" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.25">
@@ -2102,7 +2107,7 @@
       <c r="O42" s="18"/>
       <c r="P42" s="18"/>
       <c r="Q42" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R42" s="18"/>
       <c r="S42" s="18"/>
@@ -2114,7 +2119,7 @@
       <c r="Y42" s="18"/>
       <c r="Z42" s="18"/>
       <c r="AA42" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2167,34 +2172,34 @@
     <row r="45" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B47" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B48" s="16"/>
       <c r="C48" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>52</v>
@@ -2206,10 +2211,10 @@
         <v>52</v>
       </c>
       <c r="G48" s="45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="16"/>
       <c r="C49" s="27"/>
       <c r="D49" s="18"/>
@@ -2217,7 +2222,7 @@
       <c r="F49" s="18"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="16"/>
       <c r="C50" s="27"/>
       <c r="D50" s="18"/>
@@ -2225,7 +2230,7 @@
       <c r="F50" s="18"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="17"/>
       <c r="C51" s="28"/>
       <c r="D51" s="19"/>
@@ -2233,42 +2238,45 @@
       <c r="F51" s="19"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="49" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="49" t="s">
+      <c r="C55" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="H55" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="H55" s="51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="16"/>
       <c r="C56" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>54</v>
@@ -2280,10 +2288,13 @@
         <v>56</v>
       </c>
       <c r="H56" s="52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="16"/>
       <c r="C57" s="27"/>
       <c r="D57" s="27"/>
@@ -2294,9 +2305,10 @@
         <v>57</v>
       </c>
       <c r="G57" s="18"/>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="18"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="16"/>
       <c r="C58" s="27"/>
       <c r="D58" s="27"/>
@@ -2305,94 +2317,99 @@
       <c r="G58" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="18"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="16"/>
       <c r="C59" s="27"/>
       <c r="D59" s="27"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
-      <c r="H59" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="16"/>
       <c r="C60" s="27"/>
       <c r="D60" s="27"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
-      <c r="H60" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="16"/>
       <c r="C61" s="27"/>
       <c r="D61" s="27"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H61" s="18"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="17"/>
       <c r="C62" s="28"/>
       <c r="D62" s="28"/>
       <c r="E62" s="19"/>
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
     <row r="66" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B66" s="49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E66" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="G66" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H66" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G66" s="41" t="s">
+      <c r="I66" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="H66" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="I66" s="48" t="s">
+      <c r="J66" s="42" t="s">
         <v>127</v>
-      </c>
-      <c r="J66" s="42" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="D67" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
@@ -2443,7 +2460,7 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2460,31 +2477,31 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>47</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2492,7 +2509,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>56</v>
@@ -2504,7 +2521,7 @@
         <v>56</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
@@ -2516,7 +2533,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2530,7 +2547,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>

</xml_diff>

<commit_message>
new column frontend_id in token_label table
</commit_message>
<xml_diff>
--- a/DB séma train_excel.xlsx
+++ b/DB séma train_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\strabag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8468776-BA69-45B5-955A-FA99AF84CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2812B5-CFF2-4098-8030-4CE70B5E7FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="615" windowWidth="14715" windowHeight="14985" xr2:uid="{0692BD6E-48F9-45FE-A29D-EBA3E21B7AD2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0692BD6E-48F9-45FE-A29D-EBA3E21B7AD2}"/>
   </bookViews>
   <sheets>
     <sheet name="PostgreSQL" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="150">
   <si>
     <t>DB séma train_excel</t>
   </si>
@@ -83,9 +83,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>példa:</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
   </si>
   <si>
     <t xml:space="preserve">SumText </t>
+  </si>
+  <si>
+    <t>frontend_id</t>
   </si>
 </sst>
 </file>
@@ -1335,14 +1335,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2964B59E-6EC2-4CDD-BD01-A4EE83B4F2B7}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
@@ -1386,69 +1386,69 @@
     <row r="3" spans="1:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:23" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="L6" s="39" t="s">
         <v>131</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>132</v>
       </c>
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
       <c r="T6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>12</v>
@@ -1466,12 +1466,12 @@
       <c r="O7" s="47"/>
       <c r="P7" s="47"/>
       <c r="T7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>11</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="10"/>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B10" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="10"/>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="10"/>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="11"/>
@@ -1557,12 +1557,12 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1570,10 +1570,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>13</v>
@@ -1581,16 +1581,16 @@
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="I17" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K17" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="L17" s="39" t="s">
         <v>131</v>
-      </c>
-      <c r="L17" s="39" t="s">
-        <v>132</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1602,10 +1602,10 @@
         <v>3</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="47"/>
@@ -1613,13 +1613,13 @@
         <v>12</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
@@ -1627,7 +1627,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="26"/>
       <c r="E19" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="47"/>
@@ -1635,7 +1635,7 @@
         <v>11</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K19" s="18"/>
       <c r="L19" s="5"/>
@@ -1690,16 +1690,16 @@
     </row>
     <row r="24" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1716,25 +1716,25 @@
         <v>5</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N28" s="3" t="s">
+      <c r="O28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P28" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="Q28" s="2"/>
     </row>
@@ -1743,73 +1743,72 @@
         <v>5</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="38" t="s">
+      <c r="E29" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="39" t="s">
-        <v>48</v>
-      </c>
       <c r="I29" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>36</v>
-      </c>
       <c r="L29" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M29" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N29" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="5"/>
       <c r="I30" s="16"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
       <c r="M30" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N30" s="18"/>
       <c r="O30" s="5"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="5"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="5"/>
       <c r="I31" s="16"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
@@ -1819,17 +1818,14 @@
       <c r="O31" s="5"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="6"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="5"/>
       <c r="I32" s="16"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
@@ -1841,9 +1837,10 @@
     <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="10"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="5"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="5"/>
       <c r="I33" s="16"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
@@ -1855,9 +1852,10 @@
     <row r="34" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" s="10"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="5"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="5"/>
       <c r="I34" s="17"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
@@ -1869,11 +1867,12 @@
     <row r="35" spans="2:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="7"/>
       <c r="I35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1885,110 +1884,110 @@
       <c r="G38" s="18"/>
       <c r="H38" s="21"/>
       <c r="J38" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="2:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="J39" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="L39" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="M39" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="J39" s="43" t="s">
+      <c r="N39" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="K39" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="L39" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="M39" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="N39" s="3" t="s">
+      <c r="O39" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="O39" s="3" t="s">
+      <c r="P39" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="P39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="Q39" s="3" t="s">
+      <c r="R39" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="T39" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="R39" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="S39" s="3" t="s">
+      <c r="U39" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="V39" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="T39" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="U39" s="3" t="s">
+      <c r="W39" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="X39" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z39" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA39" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="V39" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="W39" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="X39" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y39" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z39" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA39" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="40" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B40" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C40" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" s="38" t="s">
+      <c r="G40" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="G40" s="38" t="s">
+      <c r="H40" s="40" t="s">
         <v>105</v>
-      </c>
-      <c r="H40" s="40" t="s">
-        <v>106</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L40" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M40" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="N40" s="18" t="s">
         <v>63</v>
-      </c>
-      <c r="N40" s="18" t="s">
-        <v>64</v>
       </c>
       <c r="O40" s="18"/>
       <c r="P40" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q40" s="18"/>
       <c r="R40" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S40" s="18"/>
       <c r="T40" s="18"/>
@@ -1996,21 +1995,21 @@
       <c r="V40" s="18"/>
       <c r="W40" s="18"/>
       <c r="X40" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y40" s="18"/>
       <c r="Z40" s="18"/>
       <c r="AA40" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B41" s="16"/>
       <c r="C41" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
@@ -2020,11 +2019,11 @@
       <c r="K41" s="24"/>
       <c r="L41" s="24"/>
       <c r="M41" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N41" s="18"/>
       <c r="O41" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P41" s="18"/>
       <c r="Q41" s="18"/>
@@ -2038,7 +2037,7 @@
       <c r="Y41" s="18"/>
       <c r="Z41" s="18"/>
       <c r="AA41" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.25">
@@ -2057,7 +2056,7 @@
       <c r="O42" s="18"/>
       <c r="P42" s="18"/>
       <c r="Q42" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R42" s="18"/>
       <c r="S42" s="18"/>
@@ -2069,7 +2068,7 @@
       <c r="Y42" s="18"/>
       <c r="Z42" s="18"/>
       <c r="AA42" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2122,46 +2121,46 @@
     <row r="45" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B47" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B48" s="16"/>
       <c r="C48" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="F48" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G48" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -2191,51 +2190,51 @@
     <row r="52" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B55" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="H55" s="45" t="s">
         <v>116</v>
-      </c>
-      <c r="H55" s="45" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="16"/>
       <c r="C56" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G56" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H56" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
@@ -2243,10 +2242,10 @@
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
       <c r="E57" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G57" s="18"/>
       <c r="H57" s="5"/>
@@ -2258,7 +2257,7 @@
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
       <c r="G58" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H58" s="5"/>
     </row>
@@ -2270,7 +2269,7 @@
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
       <c r="H59" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -2281,7 +2280,7 @@
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
       <c r="H60" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -2305,49 +2304,49 @@
     <row r="63" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
     <row r="66" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B66" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="E66" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="G66" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="H66" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G66" s="38" t="s">
+      <c r="I66" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="H66" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="I66" s="42" t="s">
+      <c r="J66" s="39" t="s">
         <v>124</v>
-      </c>
-      <c r="J66" s="39" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="D67" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
@@ -2398,7 +2397,7 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2415,31 +2414,31 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2447,23 +2446,23 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2471,7 +2470,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2485,7 +2484,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2512,31 +2511,31 @@
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
@@ -2544,7 +2543,7 @@
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13" t="s">
@@ -2576,7 +2575,7 @@
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2593,7 +2592,7 @@
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2610,7 +2609,7 @@
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>

</xml_diff>

<commit_message>
new endpoint save project
</commit_message>
<xml_diff>
--- a/DB séma train_excel.xlsx
+++ b/DB séma train_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\strabag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2812B5-CFF2-4098-8030-4CE70B5E7FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A7637F-0D07-4C41-B367-85F39AFCB219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0692BD6E-48F9-45FE-A29D-EBA3E21B7AD2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="155">
   <si>
     <t>DB séma train_excel</t>
   </si>
@@ -486,6 +486,21 @@
   </si>
   <si>
     <t>frontend_id</t>
+  </si>
+  <si>
+    <t>Projects BACKEND</t>
+  </si>
+  <si>
+    <t>TrainedProjectId</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>Trained</t>
   </si>
 </sst>
 </file>
@@ -719,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -802,6 +817,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1333,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2964B59E-6EC2-4CDD-BD01-A4EE83B4F2B7}">
-  <dimension ref="A1:AA70"/>
+  <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,6 +2394,35 @@
       <c r="J69" s="7"/>
     </row>
     <row r="70" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" s="5"/>
+    </row>
+    <row r="75" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>